<commit_message>
Deploying to main from @ pedalboard/pedalboard-display@27b15ea97f876563fadd0e18eeba4676c72a604f 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Positional/pedalboard-display-bom.xlsx
+++ b/latest/BoM/Positional/pedalboard-display-bom.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="118">
   <si>
     <t>Row</t>
   </si>
@@ -194,9 +194,6 @@
     <t>JST_PH_B3B-PH-SM4-TB_1x03-1MP_P2.00mm_Vertical</t>
   </si>
   <si>
-    <t>Connector_JST</t>
-  </si>
-  <si>
     <t>~</t>
   </si>
   <si>
@@ -296,10 +293,10 @@
     <t>OLED_128x128</t>
   </si>
   <si>
-    <t>43.2500</t>
-  </si>
-  <si>
-    <t>51.2000</t>
+    <t>49.5000</t>
+  </si>
+  <si>
+    <t>34.8000</t>
   </si>
   <si>
     <t>0.0000</t>
@@ -906,7 +903,7 @@
   <sheetData>
     <row r="1" spans="1:22" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -930,13 +927,13 @@
     </row>
     <row r="2" spans="1:22">
       <c r="C2" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>45</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F2" s="3">
         <v>6</v>
@@ -944,41 +941,41 @@
     </row>
     <row r="3" spans="1:22">
       <c r="C3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>101</v>
-      </c>
       <c r="E3" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>109</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:22">
       <c r="C4" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:22">
       <c r="C5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>105</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -986,13 +983,13 @@
     </row>
     <row r="6" spans="1:22">
       <c r="C6" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>107</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F6" s="3">
         <v>202</v>
@@ -1225,7 +1222,7 @@
         <v>57</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>43</v>
@@ -1237,25 +1234,25 @@
         <v>31</v>
       </c>
       <c r="L11" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="M11" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="M11" s="7" t="s">
+      <c r="N11" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="N11" s="5" t="s">
+      <c r="O11" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="O11" s="7" t="s">
+      <c r="P11" s="7" t="s">
         <v>62</v>
-      </c>
-      <c r="P11" s="7" t="s">
-        <v>63</v>
       </c>
       <c r="Q11" s="7" t="s">
         <v>37</v>
       </c>
       <c r="R11" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="S11" s="7" t="s">
         <v>39</v>
@@ -1264,36 +1261,36 @@
         <v>40</v>
       </c>
       <c r="U11" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="V11" s="7" t="s">
         <v>65</v>
-      </c>
-      <c r="V11" s="7" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:22">
       <c r="A12" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="C12" s="10" t="s">
         <v>68</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>69</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>55</v>
       </c>
       <c r="E12" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="G12" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="G12" s="10" t="s">
-        <v>72</v>
-      </c>
       <c r="H12" s="10" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="I12" s="8" t="s">
         <v>22</v>
@@ -1305,25 +1302,25 @@
         <v>31</v>
       </c>
       <c r="L12" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="M12" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="M12" s="10" t="s">
-        <v>60</v>
-      </c>
       <c r="N12" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="O12" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="O12" s="10" t="s">
+      <c r="P12" s="10" t="s">
         <v>74</v>
-      </c>
-      <c r="P12" s="10" t="s">
-        <v>75</v>
       </c>
       <c r="Q12" s="10" t="s">
         <v>37</v>
       </c>
       <c r="R12" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="S12" s="10" t="s">
         <v>39</v>
@@ -1332,36 +1329,36 @@
         <v>40</v>
       </c>
       <c r="U12" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="V12" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="30" customHeight="1">
       <c r="A13" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>25</v>
       </c>
       <c r="E13" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F13" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="G13" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="H13" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="I13" s="5" t="s">
         <v>22</v>
@@ -1373,22 +1370,22 @@
         <v>31</v>
       </c>
       <c r="L13" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="M13" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="N13" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O13" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="M13" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="N13" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="O13" s="7" t="s">
+      <c r="P13" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="P13" s="7" t="s">
+      <c r="Q13" s="7" t="s">
         <v>85</v>
-      </c>
-      <c r="Q13" s="7" t="s">
-        <v>86</v>
       </c>
       <c r="R13" s="7" t="s">
         <v>38</v>
@@ -1400,33 +1397,33 @@
         <v>40</v>
       </c>
       <c r="U13" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="V13" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="V13" s="7" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:22">
       <c r="A14" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>45</v>
       </c>
       <c r="E14" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" s="10" t="s">
         <v>90</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>91</v>
       </c>
       <c r="H14" s="10" t="s">
         <v>49</v>
@@ -1444,34 +1441,34 @@
         <v>23</v>
       </c>
       <c r="M14" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="N14" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="N14" s="8" t="s">
-        <v>61</v>
-      </c>
       <c r="O14" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="P14" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="P14" s="10" t="s">
+      <c r="Q14" s="10" t="s">
         <v>93</v>
-      </c>
-      <c r="Q14" s="10" t="s">
-        <v>94</v>
       </c>
       <c r="R14" s="10" t="s">
         <v>38</v>
       </c>
       <c r="S14" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="T14" s="10" t="s">
         <v>40</v>
       </c>
       <c r="U14" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="V14" s="10" t="s">
         <v>96</v>
-      </c>
-      <c r="V14" s="10" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1497,27 +1494,27 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-display@5a65175c090419f12d399ef1516610d396a1ab5b 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Positional/pedalboard-display-bom.xlsx
+++ b/latest/BoM/Positional/pedalboard-display-bom.xlsx
@@ -239,10 +239,10 @@
     <t>pedalboard-display(1)</t>
   </si>
   <si>
-    <t>107.0000</t>
-  </si>
-  <si>
-    <t>100.5500</t>
+    <t>124.0000</t>
+  </si>
+  <si>
+    <t>68.0000</t>
   </si>
   <si>
     <t>12.4000</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-display@f60ebcb4e3c80d8be295d4f5d56c3c9cb2e1f262 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Positional/pedalboard-display-bom.xlsx
+++ b/latest/BoM/Positional/pedalboard-display-bom.xlsx
@@ -271,118 +271,118 @@
     <t>https://www.passivecomponent.com/wp-content/uploads/chipR/ASC_WR.pdf</t>
   </si>
   <si>
-    <t>74.0000</t>
-  </si>
-  <si>
-    <t>102.9900</t>
+    <t>73.4000</t>
+  </si>
+  <si>
+    <t>102.5000</t>
+  </si>
+  <si>
+    <t>0.0000</t>
+  </si>
+  <si>
+    <t>1.5600</t>
+  </si>
+  <si>
+    <t>0.6400</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>U1 U2</t>
+  </si>
+  <si>
+    <t>OLED_128x128</t>
+  </si>
+  <si>
+    <t>pedalboard-display(2)</t>
+  </si>
+  <si>
+    <t>49.5000</t>
+  </si>
+  <si>
+    <t>34.8000</t>
+  </si>
+  <si>
+    <t>THT</t>
+  </si>
+  <si>
+    <t>32.1000</t>
+  </si>
+  <si>
+    <t>54.1772</t>
+  </si>
+  <si>
+    <t>KiBot Bill of Materials</t>
+  </si>
+  <si>
+    <t>Schematic:</t>
+  </si>
+  <si>
+    <t>Variant:</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>Revision:</t>
+  </si>
+  <si>
+    <t>0.0.0-RC1</t>
+  </si>
+  <si>
+    <t>Date:</t>
+  </si>
+  <si>
+    <t>2024-10-05</t>
+  </si>
+  <si>
+    <t>KiCad Version:</t>
+  </si>
+  <si>
+    <t>8.0.4+1</t>
+  </si>
+  <si>
+    <t>Component Groups:</t>
+  </si>
+  <si>
+    <t>Component Count:</t>
+  </si>
+  <si>
+    <t>202 (200 SMD/ 2 THT)</t>
+  </si>
+  <si>
+    <t>Fitted Components:</t>
+  </si>
+  <si>
+    <t>201 (199 SMD/ 2 THT)</t>
+  </si>
+  <si>
+    <t>Number of PCBs:</t>
+  </si>
+  <si>
+    <t>Total Components:</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>LED-OUT</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (DNF)</t>
+  </si>
+  <si>
+    <t>4.7000</t>
+  </si>
+  <si>
+    <t>25.0000</t>
   </si>
   <si>
     <t>270.0000</t>
-  </si>
-  <si>
-    <t>1.5600</t>
-  </si>
-  <si>
-    <t>0.6400</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>U1 U2</t>
-  </si>
-  <si>
-    <t>OLED_128x128</t>
-  </si>
-  <si>
-    <t>pedalboard-display(2)</t>
-  </si>
-  <si>
-    <t>49.5000</t>
-  </si>
-  <si>
-    <t>34.8000</t>
-  </si>
-  <si>
-    <t>0.0000</t>
-  </si>
-  <si>
-    <t>THT</t>
-  </si>
-  <si>
-    <t>32.1000</t>
-  </si>
-  <si>
-    <t>54.1772</t>
-  </si>
-  <si>
-    <t>KiBot Bill of Materials</t>
-  </si>
-  <si>
-    <t>Schematic:</t>
-  </si>
-  <si>
-    <t>Variant:</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>Revision:</t>
-  </si>
-  <si>
-    <t>0.0.0-RC1</t>
-  </si>
-  <si>
-    <t>Date:</t>
-  </si>
-  <si>
-    <t>2024-10-05</t>
-  </si>
-  <si>
-    <t>KiCad Version:</t>
-  </si>
-  <si>
-    <t>8.0.4+1</t>
-  </si>
-  <si>
-    <t>Component Groups:</t>
-  </si>
-  <si>
-    <t>Component Count:</t>
-  </si>
-  <si>
-    <t>202 (200 SMD/ 2 THT)</t>
-  </si>
-  <si>
-    <t>Fitted Components:</t>
-  </si>
-  <si>
-    <t>201 (199 SMD/ 2 THT)</t>
-  </si>
-  <si>
-    <t>Number of PCBs:</t>
-  </si>
-  <si>
-    <t>Total Components:</t>
-  </si>
-  <si>
-    <t>J2</t>
-  </si>
-  <si>
-    <t>LED-OUT</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (DNF)</t>
-  </si>
-  <si>
-    <t>4.7000</t>
-  </si>
-  <si>
-    <t>25.0000</t>
   </si>
   <si>
     <t>no</t>
@@ -984,7 +984,7 @@
   <sheetData>
     <row r="1" spans="1:22" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1008,13 +1008,13 @@
     </row>
     <row r="2" spans="1:22">
       <c r="C2" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>45</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F2" s="3">
         <v>7</v>
@@ -1022,41 +1022,41 @@
     </row>
     <row r="3" spans="1:22">
       <c r="C3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>101</v>
-      </c>
       <c r="E3" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>109</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:22">
       <c r="C4" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="E4" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>111</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:22">
       <c r="C5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>105</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1064,13 +1064,13 @@
     </row>
     <row r="6" spans="1:22">
       <c r="C6" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>107</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F6" s="3">
         <v>201</v>
@@ -1534,22 +1534,22 @@
         <v>93</v>
       </c>
       <c r="Q14" s="10" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="R14" s="10" t="s">
         <v>38</v>
       </c>
       <c r="S14" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="T14" s="10" t="s">
         <v>40</v>
       </c>
       <c r="U14" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="V14" s="10" t="s">
         <v>96</v>
-      </c>
-      <c r="V14" s="10" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1599,7 +1599,7 @@
   <sheetData>
     <row r="1" spans="1:22" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1623,13 +1623,13 @@
     </row>
     <row r="2" spans="1:22">
       <c r="C2" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>45</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F2" s="3">
         <v>7</v>
@@ -1637,41 +1637,41 @@
     </row>
     <row r="3" spans="1:22">
       <c r="C3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>101</v>
-      </c>
       <c r="E3" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>109</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:22">
       <c r="C4" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="E4" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>111</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:22">
       <c r="C5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>105</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1679,13 +1679,13 @@
     </row>
     <row r="6" spans="1:22">
       <c r="C6" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>107</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F6" s="3">
         <v>201</v>
@@ -1773,10 +1773,10 @@
         <v>55</v>
       </c>
       <c r="E9" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="F9" s="7" t="s">
         <v>115</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>116</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>58</v>
@@ -1788,10 +1788,10 @@
         <v>22</v>
       </c>
       <c r="J9" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="K9" s="5" t="s">
         <v>117</v>
-      </c>
-      <c r="K9" s="5" t="s">
-        <v>118</v>
       </c>
       <c r="L9" s="6" t="s">
         <v>59</v>
@@ -1803,13 +1803,13 @@
         <v>61</v>
       </c>
       <c r="O9" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="P9" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="P9" s="7" t="s">
+      <c r="Q9" s="7" t="s">
         <v>120</v>
-      </c>
-      <c r="Q9" s="7" t="s">
-        <v>85</v>
       </c>
       <c r="R9" s="7" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-display@ed5daf3a73271a1219396e5281b2c6e43b89c100 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Positional/pedalboard-display-bom.xlsx
+++ b/latest/BoM/Positional/pedalboard-display-bom.xlsx
@@ -211,7 +211,7 @@
     <t>87.0000</t>
   </si>
   <si>
-    <t>101.0000</t>
+    <t>83.0000</t>
   </si>
   <si>
     <t>bottom</t>
@@ -274,7 +274,7 @@
     <t>73.4000</t>
   </si>
   <si>
-    <t>102.5000</t>
+    <t>84.5000</t>
   </si>
   <si>
     <t>0.0000</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-display@a01648c17aa75a8a1f5b85c9c13e135b939d5d71 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Positional/pedalboard-display-bom.xlsx
+++ b/latest/BoM/Positional/pedalboard-display-bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="134">
   <si>
     <t>Row</t>
   </si>
@@ -211,7 +211,7 @@
     <t>87.0000</t>
   </si>
   <si>
-    <t>83.0000</t>
+    <t>78.7500</t>
   </si>
   <si>
     <t>bottom</t>
@@ -271,39 +271,42 @@
     <t>https://www.passivecomponent.com/wp-content/uploads/chipR/ASC_WR.pdf</t>
   </si>
   <si>
-    <t>73.4000</t>
-  </si>
-  <si>
-    <t>84.5000</t>
+    <t>135.4700</t>
+  </si>
+  <si>
+    <t>97.0200</t>
+  </si>
+  <si>
+    <t>270.0000</t>
+  </si>
+  <si>
+    <t>1.5600</t>
+  </si>
+  <si>
+    <t>0.6400</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>U1 U2</t>
+  </si>
+  <si>
+    <t>OLED_128x128</t>
+  </si>
+  <si>
+    <t>pedalboard-display(2)</t>
+  </si>
+  <si>
+    <t>49.5000</t>
+  </si>
+  <si>
+    <t>34.8000</t>
   </si>
   <si>
     <t>0.0000</t>
   </si>
   <si>
-    <t>1.5600</t>
-  </si>
-  <si>
-    <t>0.6400</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>U1 U2</t>
-  </si>
-  <si>
-    <t>OLED_128x128</t>
-  </si>
-  <si>
-    <t>pedalboard-display(2)</t>
-  </si>
-  <si>
-    <t>49.5000</t>
-  </si>
-  <si>
-    <t>34.8000</t>
-  </si>
-  <si>
     <t>THT</t>
   </si>
   <si>
@@ -376,13 +379,7 @@
     <t xml:space="preserve"> (DNF)</t>
   </si>
   <si>
-    <t>4.7000</t>
-  </si>
-  <si>
-    <t>25.0000</t>
-  </si>
-  <si>
-    <t>270.0000</t>
+    <t>87.2500</t>
   </si>
   <si>
     <t>no</t>
@@ -1008,7 +1005,7 @@
   <sheetData>
     <row r="1" spans="1:22" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1032,13 +1029,13 @@
     </row>
     <row r="2" spans="1:22">
       <c r="C2" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>45</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F2" s="3">
         <v>8</v>
@@ -1046,41 +1043,41 @@
     </row>
     <row r="3" spans="1:22">
       <c r="C3" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:22">
       <c r="C4" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:22">
       <c r="C5" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1088,13 +1085,13 @@
     </row>
     <row r="6" spans="1:22">
       <c r="C6" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F6" s="3">
         <v>201</v>
@@ -1558,22 +1555,22 @@
         <v>93</v>
       </c>
       <c r="Q14" s="10" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="R14" s="10" t="s">
         <v>38</v>
       </c>
       <c r="S14" s="10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="T14" s="10" t="s">
         <v>40</v>
       </c>
       <c r="U14" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="V14" s="10" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1623,7 +1620,7 @@
   <sheetData>
     <row r="1" spans="1:22" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1647,13 +1644,13 @@
     </row>
     <row r="2" spans="1:22">
       <c r="C2" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>45</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F2" s="3">
         <v>8</v>
@@ -1661,41 +1658,41 @@
     </row>
     <row r="3" spans="1:22">
       <c r="C3" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:22">
       <c r="C4" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:22">
       <c r="C5" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1703,13 +1700,13 @@
     </row>
     <row r="6" spans="1:22">
       <c r="C6" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F6" s="3">
         <v>201</v>
@@ -1797,10 +1794,10 @@
         <v>55</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>58</v>
@@ -1812,10 +1809,10 @@
         <v>22</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="L9" s="6" t="s">
         <v>59</v>
@@ -1827,13 +1824,13 @@
         <v>61</v>
       </c>
       <c r="O9" s="7" t="s">
-        <v>118</v>
+        <v>62</v>
       </c>
       <c r="P9" s="7" t="s">
         <v>119</v>
       </c>
       <c r="Q9" s="7" t="s">
-        <v>120</v>
+        <v>37</v>
       </c>
       <c r="R9" s="7" t="s">
         <v>64</v>
@@ -1842,7 +1839,7 @@
         <v>39</v>
       </c>
       <c r="T9" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="U9" s="7" t="s">
         <v>65</v>
@@ -1856,7 +1853,7 @@
         <v>43</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>77</v>
@@ -1865,13 +1862,13 @@
         <v>25</v>
       </c>
       <c r="E10" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="F10" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="G10" s="10" t="s">
         <v>124</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>125</v>
       </c>
       <c r="H10" s="10" t="s">
         <v>81</v>
@@ -1880,10 +1877,10 @@
         <v>43</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="L10" s="9" t="s">
         <v>59</v>
@@ -1895,13 +1892,13 @@
         <v>91</v>
       </c>
       <c r="O10" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="P10" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="P10" s="10" t="s">
+      <c r="Q10" s="10" t="s">
         <v>127</v>
-      </c>
-      <c r="Q10" s="10" t="s">
-        <v>128</v>
       </c>
       <c r="R10" s="10" t="s">
         <v>64</v>
@@ -1910,10 +1907,10 @@
         <v>39</v>
       </c>
       <c r="T10" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="U10" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="V10" s="10" t="s">
         <v>52</v>
@@ -1942,27 +1939,27 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-display@e0f137995197d599507c3dd5179f08441716a99e 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Positional/pedalboard-display-bom.xlsx
+++ b/latest/BoM/Positional/pedalboard-display-bom.xlsx
@@ -310,10 +310,10 @@
     <t>THT</t>
   </si>
   <si>
-    <t>32.1000</t>
-  </si>
-  <si>
-    <t>54.1772</t>
+    <t>31.7000</t>
+  </si>
+  <si>
+    <t>53.9772</t>
   </si>
   <si>
     <t>KiBot Bill of Materials</t>

</xml_diff>